<commit_message>
Att documentação, diagramas e backlog
</commit_message>
<xml_diff>
--- a/TI/ProductBacklogQualified (1).xlsx
+++ b/TI/ProductBacklogQualified (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/mauricio_martins_sptech_school/Documents/Projeto-2ºSem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathi\OneDrive\Documentos\GREENEYE-OFICIAL\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{F047EA51-ED81-470E-AFA2-2FA9EAECBE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3C53D87-DBA3-4805-88BC-8024F6D3FDC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1394DA-B463-4BCE-8B49-C4CBF0E46A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBQ" sheetId="15" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
   <si>
     <t>Product BackLog Qualified (PBQ)</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Em andamento</t>
   </si>
   <si>
-    <t>O sistema deve ter uma dashboard, que possibilite o analista monitorar todos os dados, de suas máquinas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Importante </t>
   </si>
   <si>
@@ -84,21 +81,12 @@
     <t>PROT02</t>
   </si>
   <si>
-    <t>A dashboard deve fornecer um grafíco para monitorar os dados da memória ram</t>
-  </si>
-  <si>
     <t>PROT03</t>
   </si>
   <si>
     <t>A dashboard deve fornecer um grafíco para monitorar os dados do disco</t>
   </si>
   <si>
-    <t>PROT04</t>
-  </si>
-  <si>
-    <t>A dashboard deve fornecer um grafíco para monitorar os dados da rede</t>
-  </si>
-  <si>
     <t>US002</t>
   </si>
   <si>
@@ -108,120 +96,24 @@
     <t>O sistema deve realizar um maior detalhamento do problema na abertura dos chamados</t>
   </si>
   <si>
-    <t>US003</t>
-  </si>
-  <si>
-    <t>O sistema devera ter uma aplicação, para que seja possivel a captura dos dados do hardware</t>
-  </si>
-  <si>
-    <t>Essa aplicação deve ser programada em Python ou Kotlin</t>
-  </si>
-  <si>
     <t>Em Andamento</t>
   </si>
   <si>
-    <t>Deve ser um software executável</t>
-  </si>
-  <si>
-    <t>US004</t>
-  </si>
-  <si>
     <t>Planejada</t>
   </si>
   <si>
-    <t>O sistema deve enviar alertas via Slack para os responsáveis pelo monitoramento</t>
-  </si>
-  <si>
-    <t>O slack deverá ter um grupo para os responsáveis pelo monitoramento</t>
-  </si>
-  <si>
-    <t>O sistema deverá mandar alertas quando o hardware bater metrícas de alerta</t>
-  </si>
-  <si>
     <t>US005</t>
   </si>
   <si>
-    <t>O sistema devera fornecer um monitoramento em tempo real, para que seja possivel uma melhor análise</t>
-  </si>
-  <si>
-    <t>O sistema deve capturar as métricas a cada 10 segundos e lançar no banco de dados</t>
-  </si>
-  <si>
-    <t>US006</t>
-  </si>
-  <si>
-    <t>O sistema deve capturar e enviar as métricas de forma precisa</t>
-  </si>
-  <si>
-    <t>O cliente deve ser informado sobre as métricas</t>
-  </si>
-  <si>
-    <t>O sistema deve ter uma opção de abertura de chamados</t>
-  </si>
-  <si>
     <t>US007</t>
   </si>
   <si>
-    <t>Na captura dos dados, deve ser informado a dada e o horário de cada leitura</t>
-  </si>
-  <si>
     <t>US008</t>
   </si>
   <si>
-    <t>A aplicação deverá rodar no sistema operacional Linux</t>
-  </si>
-  <si>
-    <t>A aplicação deverá rodar no sistema operacional Windows</t>
-  </si>
-  <si>
     <t>US009</t>
   </si>
   <si>
-    <t>O sistema deverá auxiliar na otimização do computador</t>
-  </si>
-  <si>
-    <t>PROT05</t>
-  </si>
-  <si>
-    <t>No site deverá conter uma tela de cadastro</t>
-  </si>
-  <si>
-    <t>PROT06</t>
-  </si>
-  <si>
-    <t>No site deverá conter uma tela de login</t>
-  </si>
-  <si>
-    <t>PROT07</t>
-  </si>
-  <si>
-    <t>No site deverá conter uma tela home</t>
-  </si>
-  <si>
-    <t>EC01</t>
-  </si>
-  <si>
-    <t>Roteiro da pesquisa</t>
-  </si>
-  <si>
-    <t>EC002</t>
-  </si>
-  <si>
-    <t>Planejamento da pesquisa</t>
-  </si>
-  <si>
-    <t>US010</t>
-  </si>
-  <si>
-    <t>O site precisa ser responsivel, tanto para computadores quanto para celulares</t>
-  </si>
-  <si>
-    <t>JU001</t>
-  </si>
-  <si>
-    <t>Diagrama de visão de negocio</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -339,43 +231,211 @@
     <t>EC</t>
   </si>
   <si>
-    <t>US011</t>
-  </si>
-  <si>
-    <t>O sistema deve ser eficiente e ceder um script para instalação da aplicação</t>
-  </si>
-  <si>
-    <t>O sistema precisa vir junto com um manual de instalação, para assim descrever os processos de instalação</t>
-  </si>
-  <si>
-    <t>US012</t>
-  </si>
-  <si>
-    <t>A nossa empresa deve promover soluções de padronização de máquinas para os nossos cllientes</t>
-  </si>
-  <si>
-    <t>US013</t>
-  </si>
-  <si>
-    <t>A aplicação deve fornecer os dados de maneira inteligente, assim facilitando a analise do analista</t>
-  </si>
-  <si>
-    <t>Não deve ser fornecido dados "inúteis", a não ser que o clliente exiga</t>
-  </si>
-  <si>
-    <t>US014</t>
-  </si>
-  <si>
-    <t>Devera ser fornecidas novas ferramentas(aplicação) para assim facilitar a manutenção das máquinas</t>
-  </si>
-  <si>
-    <t>Deve ser informado de maneira expecifica qual máquina está com defeito</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
     <t>Essencial</t>
+  </si>
+  <si>
+    <t>O sistema deve ter uma dashboard, que possibilite o técnico monitorar todos os dados de suas máquinas</t>
+  </si>
+  <si>
+    <t>Ao ser feito o monitoramento das CPUs, caso haja alguma alteração deverá ser enviado um alerta na tela para o usuário.</t>
+  </si>
+  <si>
+    <t>A dashboard deve fornecer um grafíco para monitorar os dados da memória RAM</t>
+  </si>
+  <si>
+    <t>Ao ser feito o monitoramento das RAMs, caso haja alguma alteração deverá ser enviado um alerta na tela para o usuário.</t>
+  </si>
+  <si>
+    <t>Ao ser feito o monitoramento dos Discos, caso haja alguma alteração deverá ser enviado um alerta na tela para o usuário.</t>
+  </si>
+  <si>
+    <t>Nessa seção o cliente poderá entrar em contato com nossos colaboradores 24/7 para que sejam feitos reparos ou resolução de problemas.</t>
+  </si>
+  <si>
+    <t>Ao usuário acessar a tela de dashboards o usuário terá acesso a informações especificas como cpu, memória, rede, disco etc...</t>
+  </si>
+  <si>
+    <t>PROT001</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma página de menus para a localização de mais informações sobre nossa empresa.</t>
+  </si>
+  <si>
+    <t>Ao ser acessada pelo usuário, que irá se localizar pelo menu de páginas para obter mais infomações.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de footer para que o usuário possa entrar em contato com nossa equipe.</t>
+  </si>
+  <si>
+    <t>Ao acessar as páginas do site o usuário terá de forma pratica o acesso ao footer para entrar em contato  com a equipe e tirar dúvidas.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com informações sobre o projeto.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com tópicos nos quais a equipe acredita.</t>
+  </si>
+  <si>
+    <t>PROT002</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção explicativa sobre nosso projeto, mostrando detalhes e a motivação pelo qual o projeto foi criado.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com mais detalhes sobre o projeto na tela sobre nós.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de valores para que o cliente possa ter mais detalhes e passar maior credibilidade.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com os valores dos quais movem nosso projeto e passar confiança aos nossos futuros clientes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao ser acessada a página (sobre nós) nossos usuário teram acesso a uma seção com os intergantes que pertencem a equipe e mostrar credibilidade aos clientes e usuários.  </t>
+  </si>
+  <si>
+    <t>Ao ser acessada a página (sobre nós) nossos clientes encontrarão uma seção com feedbacks de clientes que já contrataram nosso serviços, essa seção serve para que possamos ter mais credibilidade.</t>
+  </si>
+  <si>
+    <t>PROT003</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de serviços para que caso os clientes tenham interesse em nossos serviços, previamente possam nos conhecer e entrar em contato.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá uma página de serviços, onde encontrará todos os serviços realizados pela nossa empresa e o porque nos contratar.</t>
+  </si>
+  <si>
+    <t>PROT004</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o cliente terá uma página de contato, para que possa nos contactar online ou via telefones.</t>
+  </si>
+  <si>
+    <t>Ao fechar o contrato com nossa empresa, o cliente já cadastrado previamente em nossos bancos de dados possuirá uma página de login, para que possa ter acesso as dashboards relacionadas a sua empresa.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de beneficios do negócio que apresenta ao usuário como nossos serviços funcionam e no que a equipe acredita.</t>
+  </si>
+  <si>
+    <t>A página trará para os usuários informações referente ao que acreditamos e porque nossos serviços funcionam.</t>
+  </si>
+  <si>
+    <t>PROT005</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de cadastro para que o ADM possa ser cadastrado.</t>
+  </si>
+  <si>
+    <t>Essa página será utilizada pelos nossos colaboradores para realizar o cadastro dos nosso clientes em nosso banco de dados para que ele possa realizar seu login.</t>
+  </si>
+  <si>
+    <t>EC001</t>
+  </si>
+  <si>
+    <t>Essa ação consiste em realizar pesquisas com possíveis clientes e buscar problemas, falhas e desafios para que nossa equipe possa solucioná-los.</t>
+  </si>
+  <si>
+    <t>DER001</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de usuário para fazer a captura de usuários.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de perfil para para designar os niveis de permissões.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de cadastro-empresa para separar e atribuir a que empresa cada usuário pertence.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de leitura para que seja feito o armazenamento e a transformação dos dados em interface gráfica.</t>
+  </si>
+  <si>
+    <t>Ao coletar dados das máquinas esses dados serão armazenados na tabela de leitura para serem apresentados nas dashboards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O site deverá apresentar dashboards com informações dos compartimentos do sistema de forma especifica.  </t>
+  </si>
+  <si>
+    <t>A tela de ADM deverá apresentar um icone com os usuários cadastrados para que o gerente tenha acesso a quem está analisando as telas de dashboard.</t>
+  </si>
+  <si>
+    <t>A tela de usuário deverá apresentar as telas de dashboard com os componentes especificos para serem analisados.</t>
+  </si>
+  <si>
+    <t>A tela de chamado de suporte deverá apresentar cartões com os problemas para que nossa equipe possa passar para o setor responsavél.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção introdutória que apresenta inicialmente nossos serviços de forma rápida e objetiva.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção com tópicos gerais para que o usuário tenha uma visão geral sobre o que nossa equipe acredita para ter desenvolvido o projeto.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção com apresentação da equipe para que o cliente possa conhecer e ter confiança que a equipe está preparada.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de feedback para que os novos clientes e/ou usuários possam ter acesso ao feedback de empresas que já são nossos clientes;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O site deverá apresentar uma seção de contato para que o cliente tenha acesso aos nossos serviços e possa entrar em contato; </t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de login para que o cliente tenha acesso ao nosso principal serviço, sendo ele as dashboards.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de suporte para que o usuário possa ter acesso a resolução de falhas e problemas nas dashboards.</t>
+  </si>
+  <si>
+    <t>O projeto deverá ter pesquisas de campo para que a equipe possa identificar problemas, falhas e bugs nos sistemas operacionais dos totens de autoatendimento.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de lote para o controle de qual a determinada máquina pertence.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de máquina para identificação de cada máquina e que seja possível localiza-la.</t>
+  </si>
+  <si>
+    <t>Ao usuário cadastrado acessar a tela de dashboard ele terá acesso aos gráficos para fazer a analise dos componentes de sua escolha e/ou geral.</t>
+  </si>
+  <si>
+    <t>Ao ADM acessar sua tela como administrador ele terá acesso aos seus usuários cadastrados.</t>
+  </si>
+  <si>
+    <t>A tela de chamado de suporte interno deverá apresentar cartões com os problemas para que a equipe interna da empresa possa passar para o técnico responsável.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A equipe terá acesso a uma ferramenta para o gerenciamento de chamados. </t>
+  </si>
+  <si>
+    <t>Ao ser feito o cadastro pelo ADM, ele como administrador deverá ter acesso aos seus funcionários.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao ser feito o cadastro do usuário o DEV deverá conceder a permissão que o usuário terá para acessar as dashboards. </t>
+  </si>
+  <si>
+    <t>Ao ser cadastrado a empresa, o DEV irá designar a qual empresa o usuário pertence.</t>
+  </si>
+  <si>
+    <t>Ao ser feito o cadastro dos usuários, o lote cadastrado será feito pelo desenvolvedor.</t>
+  </si>
+  <si>
+    <t>Ao ser cadastrado a máquina, deve ser feito ligação com a tabela lote para especificação desses dados.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de dashboard ao Técnico, afim de visualizar os dados recebidos pela aplicação e assim ser feita a tomada de decisão dessas métricas.</t>
+  </si>
+  <si>
+    <t>O acesso a essa seção será exclusivo para os usuários que ja tiverem efetuado login, serve para que nossos clientes tenham acesso ao monitoramento de suas máquinas.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção para ADM, pois é através desta seção que o usuário administrador pode fazer a análise de relátorios e médias de suas máquinas.</t>
+  </si>
+  <si>
+    <t>Essa seção será usada pelo nosso cliente ja cadastrado em nosso banco de dados, para que ele possa ter uma base analítica sobre as médianas de seus lotes/máquinas.</t>
   </si>
 </sst>
 </file>
@@ -478,7 +538,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,12 +590,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED1458"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F3F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,23 +669,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -642,7 +687,22 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -712,19 +772,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -735,7 +795,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -747,35 +807,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -811,13 +847,38 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -844,7 +905,81 @@
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1261,22 +1396,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>80493</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>67078</xdr:rowOff>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>321972</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>404459</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1069312</xdr:rowOff>
+      <xdr:rowOff>1095375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{226EF95B-DF1B-98CF-60D3-C59EB9F2174A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A82E9D7-5A94-F485-9514-9D2F919DDCE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1284,16 +1419,15 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect t="33824" b="38603"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="335387" y="281726"/>
-          <a:ext cx="1086655" cy="1002234"/>
+          <a:off x="752476" y="190500"/>
+          <a:ext cx="4041648" cy="1114425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1627,893 +1761,935 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:I51"/>
+  <dimension ref="B1:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="131.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="51.5703125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="3.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="131.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="51.5546875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+    <row r="1" spans="2:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
       <c r="I2"/>
     </row>
-    <row r="3" spans="2:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="2:9" s="25" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="45" t="s">
+    <row r="3" spans="2:9" s="25" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="38">
+    <row r="4" spans="2:9" s="26" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30">
         <v>1</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="30">
+        <v>2</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34">
+        <v>3</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="30">
+        <v>4</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="30">
+        <v>5</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="30">
+        <v>6</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <v>7</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="G10" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="30">
+        <v>8</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="30">
+        <v>9</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="38">
-        <v>2</v>
-      </c>
-      <c r="C6" s="41" t="s">
+      <c r="F12" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
+        <v>10</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
         <v>11</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="C14" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="26" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
         <v>12</v>
       </c>
-      <c r="F6" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="40"/>
-    </row>
-    <row r="7" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="42">
-        <v>3</v>
-      </c>
-      <c r="C7" s="41" t="s">
+      <c r="C15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="26" customFormat="1" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="30">
         <v>13</v>
       </c>
-      <c r="D7" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="40" t="s">
+      <c r="C16" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" s="26" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30">
         <v>14</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="38">
-        <v>4</v>
-      </c>
-      <c r="C8" s="41" t="s">
+      <c r="C17" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="26" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="30">
         <v>15</v>
       </c>
-      <c r="D8" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="40" t="s">
+      <c r="C18" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="40"/>
-    </row>
-    <row r="9" spans="2:9" s="26" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="38">
-        <v>3</v>
-      </c>
-      <c r="C9" s="41" t="s">
+      <c r="E18" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="26" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="30">
+        <v>16</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="30">
         <v>17</v>
       </c>
-      <c r="D9" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="40" t="s">
+      <c r="C20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="30">
         <v>18</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="40"/>
-    </row>
-    <row r="10" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="38">
-        <v>4</v>
-      </c>
-      <c r="C10" s="38" t="s">
+      <c r="C21" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="26" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="30">
         <v>19</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="C22" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="26" customFormat="1" ht="91.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="30">
         <v>20</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="C23" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="26" customFormat="1" ht="91.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="30">
         <v>21</v>
       </c>
-      <c r="F10" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="40"/>
-    </row>
-    <row r="11" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="38">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42" t="s">
+      <c r="C24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="26" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="30">
         <v>22</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="C25" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="30">
+        <v>23</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="30">
+        <v>24</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="30">
+        <v>25</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" s="26" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="30">
+        <v>26</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="30">
+        <v>27</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="30">
+        <v>28</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="30">
+        <v>29</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="D32" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" s="15" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="33">
+        <v>30</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" s="15" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="33">
+        <v>31</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" s="15" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="33">
+        <v>32</v>
+      </c>
+      <c r="C35" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="40"/>
-    </row>
-    <row r="12" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="38">
-        <v>6</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="40"/>
-    </row>
-    <row r="13" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="38">
-        <v>7</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" s="40"/>
-    </row>
-    <row r="14" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="38">
-        <v>8</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="40"/>
-    </row>
-    <row r="15" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="38">
-        <v>9</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G15" s="40"/>
-    </row>
-    <row r="16" spans="2:9" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="38">
-        <v>10</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="40"/>
-    </row>
-    <row r="17" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="38">
-        <v>11</v>
-      </c>
-      <c r="C17" s="38" t="s">
+      <c r="D35" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" s="15" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="33">
         <v>32</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="39" t="s">
+      <c r="C36" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" s="40"/>
-    </row>
-    <row r="18" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="38">
-        <v>12</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
-        <v>13</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="40"/>
-    </row>
-    <row r="20" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
-        <v>14</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="40"/>
-    </row>
-    <row r="21" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
-        <v>15</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="40"/>
-    </row>
-    <row r="22" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
-        <v>16</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="40"/>
-    </row>
-    <row r="23" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="38">
-        <v>17</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="40"/>
-    </row>
-    <row r="24" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="38">
-        <v>18</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" s="40"/>
-    </row>
-    <row r="25" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="38">
-        <v>19</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="40"/>
-    </row>
-    <row r="26" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="38">
-        <v>20</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="40"/>
-    </row>
-    <row r="27" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="38">
-        <v>21</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="40"/>
-    </row>
-    <row r="28" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="38">
-        <v>22</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" s="40"/>
-    </row>
-    <row r="29" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="38">
-        <v>23</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="40"/>
-    </row>
-    <row r="30" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="38">
-        <v>24</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G30" s="40"/>
-    </row>
-    <row r="31" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="38">
-        <v>25</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G31" s="40"/>
-    </row>
-    <row r="32" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="38">
-        <v>26</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="40"/>
-    </row>
-    <row r="33" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="38">
-        <v>27</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="40"/>
-    </row>
-    <row r="34" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="38">
-        <v>28</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="40"/>
-    </row>
-    <row r="35" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="41">
-        <v>29</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="40"/>
-    </row>
-    <row r="36" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="41">
-        <v>30</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G36" s="40"/>
-    </row>
-    <row r="37" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="41">
-        <v>31</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="F37" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G37" s="40"/>
-    </row>
-    <row r="38" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="41">
-        <v>32</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G38" s="40"/>
-    </row>
-    <row r="39" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="41">
-        <v>33</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="40"/>
-    </row>
-    <row r="40" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="40"/>
-    </row>
-    <row r="41" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="F40" s="16"/>
+    </row>
+    <row r="41" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
       <c r="F42" s="16"/>
     </row>
-    <row r="43" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+    <row r="46" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
+    <row r="47" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="F48" s="16"/>
-    </row>
-    <row r="49" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="F49" s="16"/>
-    </row>
-    <row r="50" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F50" s="16"/>
-    </row>
-    <row r="51" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F51" s="16"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
-  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="D5:E5 G20:G34 G5 C13:E13 D14:D34">
-    <cfRule type="expression" dxfId="38" priority="59">
-      <formula>$D5="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="60">
-      <formula>$D5="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="61">
-      <formula>$D5="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="62">
-      <formula>$D5="Dropped"</formula>
+  <conditionalFormatting sqref="D4:E4 G18:G32 G4 C11:E11 D12:D32">
+    <cfRule type="expression" dxfId="47" priority="59">
+      <formula>$D4="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="60">
+      <formula>$D4="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="61">
+      <formula>$D4="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="62">
+      <formula>$D4="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C19 B20:C34 E14:E34">
-    <cfRule type="expression" dxfId="34" priority="26">
-      <formula>$D$4="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="31">
-      <formula>$D14="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
-      <formula>$D14="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
-      <formula>$D14="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="34">
-      <formula>$D14="Dropped"</formula>
+  <conditionalFormatting sqref="C12:C17 B18:C32 E12:E32">
+    <cfRule type="expression" dxfId="43" priority="26">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="31">
+      <formula>$D12="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="32">
+      <formula>$D12="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="33">
+      <formula>$D12="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="34">
+      <formula>$D12="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="29" priority="22">
-      <formula>$D5="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="23">
-      <formula>$D5="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="24">
-      <formula>$D5="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="25">
-      <formula>$D5="Dropped"</formula>
+  <conditionalFormatting sqref="B4:C4">
+    <cfRule type="expression" dxfId="38" priority="22">
+      <formula>$D4="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="23">
+      <formula>$D4="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="24">
+      <formula>$D4="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="25">
+      <formula>$D4="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G12 B6:B7">
-    <cfRule type="expression" dxfId="25" priority="79">
+  <conditionalFormatting sqref="B5:B6 G5:G7">
+    <cfRule type="expression" dxfId="34" priority="79">
+      <formula>$D11="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="80">
+      <formula>$D11="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="81">
+      <formula>$D11="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="82">
+      <formula>$D11="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G17">
+    <cfRule type="expression" dxfId="30" priority="83">
+      <formula>#REF!="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="84">
+      <formula>#REF!="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="85">
+      <formula>#REF!="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="86">
+      <formula>#REF!="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10">
+    <cfRule type="expression" dxfId="26" priority="135">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="136">
+      <formula>$D15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="137">
+      <formula>$D15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="138">
+      <formula>$D15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="139">
+      <formula>$D15="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B17">
+    <cfRule type="expression" dxfId="21" priority="140">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="141">
+      <formula>#REF!="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="142">
+      <formula>#REF!="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="143">
+      <formula>#REF!="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="144">
+      <formula>#REF!="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:E8">
+    <cfRule type="expression" dxfId="16" priority="5">
+      <formula>$D8="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="6">
+      <formula>$D8="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>$D8="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="8">
+      <formula>$D8="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:E9">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>$D9="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>$D9="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>$D9="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>$D9="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G10">
+    <cfRule type="expression" dxfId="8" priority="164">
+      <formula>$D15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="165">
+      <formula>$D15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="166">
+      <formula>$D15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="167">
+      <formula>$D15="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="4" priority="168">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="169">
       <formula>$D13="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="80">
+    <cfRule type="expression" dxfId="2" priority="170">
       <formula>$D13="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="81">
+    <cfRule type="expression" dxfId="1" priority="171">
       <formula>$D13="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="82">
+    <cfRule type="expression" dxfId="0" priority="172">
       <formula>$D13="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13:G19">
-    <cfRule type="expression" dxfId="21" priority="83">
-      <formula>#REF!="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="84">
-      <formula>#REF!="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="85">
-      <formula>#REF!="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="86">
-      <formula>#REF!="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B12">
-    <cfRule type="expression" dxfId="17" priority="135">
-      <formula>$D$4="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="136">
-      <formula>$D15="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="137">
-      <formula>$D15="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="138">
-      <formula>$D15="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="139">
-      <formula>$D15="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B19">
-    <cfRule type="expression" dxfId="12" priority="140">
-      <formula>$D$4="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="141">
-      <formula>#REF!="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="142">
-      <formula>#REF!="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="143">
-      <formula>#REF!="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="144">
-      <formula>#REF!="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:E10">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$D10="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$D10="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$D10="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>$D10="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:E11">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$D11="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$D11="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$D11="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$D11="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2526,7 +2702,7 @@
           <x14:formula1>
             <xm:f>Dados!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D5 D10:D11 D13:D34</xm:sqref>
+          <xm:sqref>D4 D8:D9 D11:D32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2542,251 +2718,251 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2"/>
-    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="2" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="2"/>
+    <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="23" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="47">
+        <v>27</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="39">
         <v>1</v>
       </c>
-      <c r="H2" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="47">
+        <v>30</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="39">
         <v>2</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="47">
+        <v>32</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="39">
         <v>3</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2805,21 +2981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD94351161D70F4CAEBD7B86231B3DDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1125e75a947c6aa242f32189ae53cd99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c622a8eb0fdcb94016562c81bc647671" ns3:_="">
     <xsd:import namespace="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
@@ -2991,31 +3152,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{073EAB6A-72FD-475B-BA3D-38768563A2A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3031,4 +3183,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
att documentação e equipe
</commit_message>
<xml_diff>
--- a/TI/ProductBacklogQualified (1).xlsx
+++ b/TI/ProductBacklogQualified (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathi\OneDrive\Documentos\GREENEYE-OFICIAL\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1394DA-B463-4BCE-8B49-C4CBF0E46A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87ACDCF-EE38-44DA-8112-CCFAA06748FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBQ" sheetId="15" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="156">
   <si>
     <t>Product BackLog Qualified (PBQ)</t>
   </si>
@@ -66,9 +66,6 @@
     <t>US001</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
     <t xml:space="preserve">Importante </t>
   </si>
   <si>
@@ -432,10 +429,85 @@
     <t>O acesso a essa seção será exclusivo para os usuários que ja tiverem efetuado login, serve para que nossos clientes tenham acesso ao monitoramento de suas máquinas.</t>
   </si>
   <si>
-    <t>O site deverá apresentar uma seção para ADM, pois é através desta seção que o usuário administrador pode fazer a análise de relátorios e médias de suas máquinas.</t>
-  </si>
-  <si>
     <t>Essa seção será usada pelo nosso cliente ja cadastrado em nosso banco de dados, para que ele possa ter uma base analítica sobre as médianas de seus lotes/máquinas.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>3.2.4</t>
+  </si>
+  <si>
+    <t>3.2.5</t>
+  </si>
+  <si>
+    <t>3.2.6</t>
+  </si>
+  <si>
+    <t>3.2.7</t>
+  </si>
+  <si>
+    <t>3.2.8</t>
+  </si>
+  <si>
+    <t>3.2.9</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de login para ADM (Administrador), pois é através desta seção que o usuário administrador pode fazer a análise de relátorios e médias de suas máquinas.</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
   </si>
 </sst>
 </file>
@@ -856,12 +928,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -879,6 +945,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -905,7 +977,49 @@
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="53">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1763,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:H37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1783,14 +1897,14 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
       <c r="I2"/>
     </row>
     <row r="3" spans="2:9" s="25" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1806,671 +1920,671 @@
       <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="48" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="26" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="30">
         <v>1</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="26" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="31" t="s">
+      <c r="D5" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30">
-        <v>2</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="32" t="s">
+    </row>
+    <row r="7" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="45" t="s">
+      <c r="D7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34">
-        <v>3</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="F7" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="45" t="s">
+      <c r="D8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30">
-        <v>4</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="30">
-        <v>5</v>
-      </c>
-      <c r="C8" s="30" t="s">
+    <row r="9" spans="2:9" s="15" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30">
-        <v>6</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>74</v>
+      <c r="E9" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="30">
-        <v>7</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>75</v>
-      </c>
       <c r="F10" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="30">
+        <v>3</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="46" t="s">
+      <c r="G12" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="45" t="s">
+      <c r="F14" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30">
-        <v>9</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="46" t="s">
+    <row r="15" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" s="26" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="45" t="s">
+      <c r="F17" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="26" customFormat="1" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" s="26" customFormat="1" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="30">
-        <v>10</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="30">
-        <v>11</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" s="26" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="30">
-        <v>12</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="46" t="s">
+      <c r="D18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="45" t="s">
+      <c r="F18" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="43" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="2:9" s="26" customFormat="1" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="30">
-        <v>13</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="46" t="s">
+    <row r="19" spans="2:7" s="26" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="26" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" s="26" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="30">
-        <v>14</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="45" t="s">
+      <c r="F20" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="26" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" s="26" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="30">
+      <c r="D21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="46" t="s">
+      <c r="E21" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="F18" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="45" t="s">
+      <c r="F21" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="26" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="30">
-        <v>16</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="46" t="s">
+    <row r="22" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="30">
+        <v>4</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="15" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="26" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="26" customFormat="1" ht="91.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="30">
+        <v>5</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="30">
-        <v>17</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="45" t="s">
+      <c r="F26" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="15" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="15" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" s="26" customFormat="1" ht="91.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="30">
+        <v>6</v>
+      </c>
+      <c r="C29" s="30" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="30">
-        <v>18</v>
-      </c>
-      <c r="C21" s="30" t="s">
+      <c r="D29" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" s="26" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="30">
-        <v>19</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" s="26" customFormat="1" ht="91.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="30">
-        <v>20</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="46" t="s">
+      <c r="F29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" s="26" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="30">
+        <v>7</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" s="26" customFormat="1" ht="91.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="30">
-        <v>21</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" s="26" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="30">
-        <v>22</v>
-      </c>
-      <c r="C25" s="30" t="s">
+      <c r="F30" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="46" t="s">
+    </row>
+    <row r="31" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="30">
+        <v>8</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" s="26" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="45" t="s">
+      <c r="F35" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="30" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="30">
-        <v>23</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="30">
-        <v>24</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" s="26" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="30">
-        <v>25</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="45" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" s="26" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="30">
-        <v>26</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="30">
-        <v>27</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="31" t="s">
+      <c r="D36" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="45" t="s">
+      <c r="F36" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="43" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="30">
-        <v>28</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" s="26" customFormat="1" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="30">
-        <v>29</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" s="15" customFormat="1" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="33">
-        <v>30</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" s="15" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33">
-        <v>31</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" s="15" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="33">
-        <v>32</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" s="15" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="33">
-        <v>32</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="45" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="37" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2526,170 +2640,187 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="D4:E4 G18:G32 G4 C11:E11 D12:D32">
-    <cfRule type="expression" dxfId="47" priority="59">
+  <conditionalFormatting sqref="D5:E5 C13:E13 G4:G5 D4 G20:G23 D14:D23 D25:D26 G25:G26 G29:G36 D29:D36">
+    <cfRule type="expression" dxfId="52" priority="64">
       <formula>$D4="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="60">
+    <cfRule type="expression" dxfId="51" priority="65">
       <formula>$D4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="61">
+    <cfRule type="expression" dxfId="50" priority="66">
       <formula>$D4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="62">
+    <cfRule type="expression" dxfId="49" priority="67">
       <formula>$D4="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C17 B18:C32 E12:E32">
-    <cfRule type="expression" dxfId="43" priority="26">
+  <conditionalFormatting sqref="C14:C19 B20:C23 E14:E23 E25:E26 B25:C26 B29:C36 E29:E36">
+    <cfRule type="expression" dxfId="48" priority="31">
       <formula>$D$3="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="31">
-      <formula>$D12="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="32">
-      <formula>$D12="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="33">
-      <formula>$D12="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="34">
-      <formula>$D12="Dropped"</formula>
+    <cfRule type="expression" dxfId="47" priority="36">
+      <formula>$D14="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="37">
+      <formula>$D14="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="38">
+      <formula>$D14="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="39">
+      <formula>$D14="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4">
-    <cfRule type="expression" dxfId="38" priority="22">
+  <conditionalFormatting sqref="B5:C5">
+    <cfRule type="expression" dxfId="43" priority="27">
+      <formula>$D5="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="28">
+      <formula>$D5="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="29">
+      <formula>$D5="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="30">
+      <formula>$D5="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B7 G6:G8">
+    <cfRule type="expression" dxfId="39" priority="84">
+      <formula>$D13="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="85">
+      <formula>$D13="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="86">
+      <formula>$D13="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="87">
+      <formula>$D13="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G19">
+    <cfRule type="expression" dxfId="35" priority="88">
+      <formula>#REF!="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="89">
+      <formula>#REF!="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="90">
+      <formula>#REF!="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="91">
+      <formula>#REF!="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B12">
+    <cfRule type="expression" dxfId="31" priority="140">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="141">
+      <formula>$D17="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="142">
+      <formula>$D17="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="143">
+      <formula>$D17="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="144">
+      <formula>$D17="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B19">
+    <cfRule type="expression" dxfId="26" priority="145">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="146">
+      <formula>#REF!="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="147">
+      <formula>#REF!="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="148">
+      <formula>#REF!="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="149">
+      <formula>#REF!="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="expression" dxfId="21" priority="10">
+      <formula>$D10="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="11">
+      <formula>$D10="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="12">
+      <formula>$D10="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="13">
+      <formula>$D10="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E11">
+    <cfRule type="expression" dxfId="17" priority="6">
+      <formula>$D11="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="7">
+      <formula>$D11="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="8">
+      <formula>$D11="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="9">
+      <formula>$D11="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:G12">
+    <cfRule type="expression" dxfId="13" priority="169">
+      <formula>$D17="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="170">
+      <formula>$D17="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="171">
+      <formula>$D17="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="172">
+      <formula>$D17="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="9" priority="173">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="174">
+      <formula>$D15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="175">
+      <formula>$D15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="176">
+      <formula>$D15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="177">
+      <formula>$D15="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:C4 E4">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$D$3="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D4="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$D4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="25">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$D4="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B6 G5:G7">
-    <cfRule type="expression" dxfId="34" priority="79">
-      <formula>$D11="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="80">
-      <formula>$D11="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="81">
-      <formula>$D11="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="82">
-      <formula>$D11="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G17">
-    <cfRule type="expression" dxfId="30" priority="83">
-      <formula>#REF!="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="84">
-      <formula>#REF!="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="85">
-      <formula>#REF!="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="86">
-      <formula>#REF!="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10">
-    <cfRule type="expression" dxfId="26" priority="135">
-      <formula>$D$3="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="136">
-      <formula>$D15="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="137">
-      <formula>$D15="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="138">
-      <formula>$D15="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="139">
-      <formula>$D15="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B17">
-    <cfRule type="expression" dxfId="21" priority="140">
-      <formula>$D$3="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="141">
-      <formula>#REF!="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="142">
-      <formula>#REF!="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="143">
-      <formula>#REF!="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="144">
-      <formula>#REF!="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:E8">
-    <cfRule type="expression" dxfId="16" priority="5">
-      <formula>$D8="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
-      <formula>$D8="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula>$D8="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8">
-      <formula>$D8="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:E9">
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>$D9="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>$D9="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3">
-      <formula>$D9="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>$D9="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G10">
-    <cfRule type="expression" dxfId="8" priority="164">
-      <formula>$D15="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="165">
-      <formula>$D15="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="166">
-      <formula>$D15="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="167">
-      <formula>$D15="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="4" priority="168">
-      <formula>$D$3="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="169">
-      <formula>$D13="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="170">
-      <formula>$D13="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="171">
-      <formula>$D13="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="172">
-      <formula>$D13="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2702,7 +2833,7 @@
           <x14:formula1>
             <xm:f>Dados!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D4 D8:D9 D11:D32</xm:sqref>
+          <xm:sqref>D4:D5 D10:D11 D13:D23 D25:D26 D29:D36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2734,10 +2865,10 @@
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -2746,33 +2877,33 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="E2" s="38" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>28</v>
       </c>
       <c r="F2" s="39">
         <v>1</v>
       </c>
-      <c r="H2" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="H2" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="39">
         <v>2</v>
@@ -2784,13 +2915,13 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="E4" s="38" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>33</v>
       </c>
       <c r="F4" s="39">
         <v>3</v>
@@ -2802,22 +2933,22 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+        <v>33</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="13"/>
     </row>
@@ -2825,28 +2956,28 @@
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2871,98 +3002,98 @@
     </row>
     <row r="16" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2981,6 +3112,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD94351161D70F4CAEBD7B86231B3DDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1125e75a947c6aa242f32189ae53cd99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c622a8eb0fdcb94016562c81bc647671" ns3:_="">
     <xsd:import namespace="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
@@ -3152,22 +3298,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{073EAB6A-72FD-475B-BA3D-38768563A2A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3183,28 +3338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>